<commit_message>
deletes unnecessary created files
</commit_message>
<xml_diff>
--- a/both.xlsx
+++ b/both.xlsx
@@ -671,25 +671,25 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -734,25 +734,25 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -1301,25 +1301,25 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" t="n">
         <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" t="n">
         <v>0</v>
@@ -1364,7 +1364,7 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
         <v>4</v>
@@ -1616,25 +1616,25 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" t="n">
         <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" t="n">
         <v>0</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" t="n">
         <v>1</v>
@@ -1679,25 +1679,25 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
         <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" t="n">
         <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
         <v>1</v>
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H22" t="n">
         <v>1</v>
@@ -2183,7 +2183,7 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H29" t="n">
         <v>1</v>
@@ -2246,7 +2246,7 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -2553,7 +2553,7 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H35" t="n">
         <v>1</v>
@@ -2616,25 +2616,25 @@
         </is>
       </c>
       <c r="G36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H36" t="n">
         <v>2</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="n">
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" t="n">
         <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N36" t="n">
         <v>-1</v>
@@ -2679,7 +2679,7 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H37" t="n">
         <v>2</v>
@@ -2931,7 +2931,7 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H41" t="n">
         <v>2</v>
@@ -3057,7 +3057,7 @@
         </is>
       </c>
       <c r="G43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H43" t="n">
         <v>2</v>
@@ -3309,7 +3309,7 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H47" t="n">
         <v>3</v>
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="G48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H48" t="n">
         <v>3</v>
@@ -3435,7 +3435,7 @@
         </is>
       </c>
       <c r="G49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H49" t="n">
         <v>2</v>
@@ -3444,13 +3444,13 @@
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49" t="n">
         <v>0</v>
@@ -3750,7 +3750,7 @@
         </is>
       </c>
       <c r="G54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H54" t="n">
         <v>3</v>
@@ -3813,25 +3813,25 @@
         </is>
       </c>
       <c r="G55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H55" t="n">
         <v>1</v>
       </c>
       <c r="I55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" t="n">
         <v>0</v>
       </c>
       <c r="K55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55" t="n">
         <v>0</v>
       </c>
       <c r="M55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N55" t="n">
         <v>0</v>
@@ -3876,7 +3876,7 @@
         </is>
       </c>
       <c r="G56" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H56" t="n">
         <v>2</v>
@@ -3939,7 +3939,7 @@
         </is>
       </c>
       <c r="G57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H57" t="n">
         <v>2</v>
@@ -4002,7 +4002,7 @@
         </is>
       </c>
       <c r="G58" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H58" t="n">
         <v>3</v>
@@ -4011,13 +4011,13 @@
         <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M58" t="n">
         <v>0</v>
@@ -4128,7 +4128,7 @@
         </is>
       </c>
       <c r="G60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -4191,7 +4191,7 @@
         </is>
       </c>
       <c r="G61" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H61" t="n">
         <v>1</v>
@@ -4317,7 +4317,7 @@
         </is>
       </c>
       <c r="G63" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H63" t="n">
         <v>1</v>
@@ -4506,7 +4506,7 @@
         </is>
       </c>
       <c r="G66" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H66" t="n">
         <v>3</v>
@@ -4632,7 +4632,7 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -4758,7 +4758,7 @@
         </is>
       </c>
       <c r="G70" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H70" t="n">
         <v>1</v>
@@ -5262,7 +5262,7 @@
         </is>
       </c>
       <c r="G78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H78" t="n">
         <v>2</v>
@@ -5271,13 +5271,13 @@
         <v>0</v>
       </c>
       <c r="J78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M78" t="n">
         <v>0</v>
@@ -5449,7 +5449,7 @@
         </is>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H81" t="n">
         <v>2</v>
@@ -5458,13 +5458,13 @@
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M81" t="n">
         <v>0</v>
@@ -5512,7 +5512,7 @@
         </is>
       </c>
       <c r="G82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H82" t="n">
         <v>1</v>
@@ -5575,25 +5575,25 @@
         </is>
       </c>
       <c r="G83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H83" t="n">
         <v>1</v>
       </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J83" t="n">
         <v>0</v>
       </c>
       <c r="K83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L83" t="n">
         <v>0</v>
       </c>
       <c r="M83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N83" t="n">
         <v>4</v>
@@ -5827,25 +5827,25 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H87" t="n">
         <v>1</v>
       </c>
       <c r="I87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J87" t="n">
         <v>0</v>
       </c>
       <c r="K87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L87" t="n">
         <v>0</v>
       </c>
       <c r="M87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N87" t="n">
         <v>-1</v>
@@ -5890,25 +5890,25 @@
         </is>
       </c>
       <c r="G88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H88" t="n">
         <v>2</v>
       </c>
       <c r="I88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J88" t="n">
         <v>0</v>
       </c>
       <c r="K88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L88" t="n">
         <v>0</v>
       </c>
       <c r="M88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N88" t="n">
         <v>-3</v>
@@ -5953,7 +5953,7 @@
         </is>
       </c>
       <c r="G89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H89" t="n">
         <v>2</v>
@@ -5962,13 +5962,13 @@
         <v>0</v>
       </c>
       <c r="J89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M89" t="n">
         <v>0</v>
@@ -6079,7 +6079,7 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H91" t="n">
         <v>3</v>
@@ -6088,13 +6088,13 @@
         <v>0</v>
       </c>
       <c r="J91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M91" t="n">
         <v>0</v>
@@ -6268,25 +6268,25 @@
         </is>
       </c>
       <c r="G94" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H94" t="n">
         <v>1</v>
       </c>
       <c r="I94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J94" t="n">
         <v>0</v>
       </c>
       <c r="K94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L94" t="n">
         <v>0</v>
       </c>
       <c r="M94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N94" t="n">
         <v>0</v>
@@ -6331,7 +6331,7 @@
         </is>
       </c>
       <c r="G95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H95" t="n">
         <v>3</v>
@@ -6583,7 +6583,7 @@
         </is>
       </c>
       <c r="G99" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -7276,25 +7276,25 @@
         </is>
       </c>
       <c r="G110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H110" t="n">
         <v>1</v>
       </c>
       <c r="I110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J110" t="n">
         <v>0</v>
       </c>
       <c r="K110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L110" t="n">
         <v>0</v>
       </c>
       <c r="M110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N110" t="n">
         <v>0</v>
@@ -7465,25 +7465,25 @@
         </is>
       </c>
       <c r="G113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H113" t="n">
         <v>1</v>
       </c>
       <c r="I113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J113" t="n">
         <v>0</v>
       </c>
       <c r="K113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L113" t="n">
         <v>0</v>
       </c>
       <c r="M113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N113" t="n">
         <v>-1</v>
@@ -7528,25 +7528,25 @@
         </is>
       </c>
       <c r="G114" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H114" t="n">
         <v>1</v>
       </c>
       <c r="I114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J114" t="n">
         <v>0</v>
       </c>
       <c r="K114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L114" t="n">
         <v>0</v>
       </c>
       <c r="M114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N114" t="n">
         <v>4</v>
@@ -7654,25 +7654,25 @@
         </is>
       </c>
       <c r="G116" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H116" t="n">
         <v>4</v>
       </c>
       <c r="I116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J116" t="n">
         <v>0</v>
       </c>
       <c r="K116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L116" t="n">
         <v>0</v>
       </c>
       <c r="M116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N116" t="n">
         <v>-2</v>
@@ -7843,25 +7843,25 @@
         </is>
       </c>
       <c r="G119" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H119" t="n">
         <v>1</v>
       </c>
       <c r="I119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J119" t="n">
         <v>0</v>
       </c>
       <c r="K119" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L119" t="n">
         <v>0</v>
       </c>
       <c r="M119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N119" t="n">
         <v>-1</v>
@@ -8154,7 +8154,7 @@
         </is>
       </c>
       <c r="G124" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -8343,7 +8343,7 @@
         </is>
       </c>
       <c r="G127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H127" t="n">
         <v>2</v>
@@ -8352,13 +8352,13 @@
         <v>0</v>
       </c>
       <c r="J127" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L127" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M127" t="n">
         <v>0</v>
@@ -8406,25 +8406,25 @@
         </is>
       </c>
       <c r="G128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H128" t="n">
         <v>1</v>
       </c>
       <c r="I128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J128" t="n">
         <v>0</v>
       </c>
       <c r="K128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L128" t="n">
         <v>0</v>
       </c>
       <c r="M128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N128" t="n">
         <v>2</v>
@@ -8469,7 +8469,7 @@
         </is>
       </c>
       <c r="G129" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H129" t="n">
         <v>2</v>
@@ -8478,13 +8478,13 @@
         <v>0</v>
       </c>
       <c r="J129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M129" t="n">
         <v>0</v>
@@ -8654,25 +8654,25 @@
         </is>
       </c>
       <c r="G132" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H132" t="n">
         <v>1</v>
       </c>
       <c r="I132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J132" t="n">
         <v>0</v>
       </c>
       <c r="K132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L132" t="n">
         <v>0</v>
       </c>
       <c r="M132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N132" t="n">
         <v>2</v>
@@ -9095,7 +9095,7 @@
         </is>
       </c>
       <c r="G139" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H139" t="n">
         <v>2</v>
@@ -9104,13 +9104,13 @@
         <v>0</v>
       </c>
       <c r="J139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K139" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M139" t="n">
         <v>0</v>
@@ -9221,7 +9221,7 @@
         </is>
       </c>
       <c r="G141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H141" t="n">
         <v>1</v>
@@ -9230,13 +9230,13 @@
         <v>0</v>
       </c>
       <c r="J141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M141" t="n">
         <v>0</v>
@@ -9284,7 +9284,7 @@
         </is>
       </c>
       <c r="G142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H142" t="n">
         <v>4</v>
@@ -9536,7 +9536,7 @@
         </is>
       </c>
       <c r="G146" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H146" t="n">
         <v>3</v>
@@ -9599,25 +9599,25 @@
         </is>
       </c>
       <c r="G147" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H147" t="n">
         <v>2</v>
       </c>
       <c r="I147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J147" t="n">
         <v>0</v>
       </c>
       <c r="K147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L147" t="n">
         <v>0</v>
       </c>
       <c r="M147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N147" t="n">
         <v>-2</v>
@@ -9977,25 +9977,25 @@
         </is>
       </c>
       <c r="G153" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H153" t="n">
         <v>1</v>
       </c>
       <c r="I153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J153" t="n">
         <v>0</v>
       </c>
       <c r="K153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L153" t="n">
         <v>0</v>
       </c>
       <c r="M153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N153" t="n">
         <v>0</v>
@@ -10040,7 +10040,7 @@
         </is>
       </c>
       <c r="G154" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H154" t="n">
         <v>0</v>
@@ -10418,25 +10418,25 @@
         </is>
       </c>
       <c r="G160" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H160" t="n">
         <v>1</v>
       </c>
       <c r="I160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J160" t="n">
         <v>0</v>
       </c>
       <c r="K160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L160" t="n">
         <v>0</v>
       </c>
       <c r="M160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N160" t="n">
         <v>2</v>
@@ -10542,7 +10542,7 @@
         </is>
       </c>
       <c r="G162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H162" t="n">
         <v>4</v>
@@ -10792,25 +10792,25 @@
         </is>
       </c>
       <c r="G166" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H166" t="n">
         <v>1</v>
       </c>
       <c r="I166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J166" t="n">
         <v>0</v>
       </c>
       <c r="K166" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L166" t="n">
         <v>0</v>
       </c>
       <c r="M166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N166" t="n">
         <v>1</v>
@@ -10855,25 +10855,25 @@
         </is>
       </c>
       <c r="G167" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H167" t="n">
         <v>1</v>
       </c>
       <c r="I167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J167" t="n">
         <v>0</v>
       </c>
       <c r="K167" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L167" t="n">
         <v>0</v>
       </c>
       <c r="M167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N167" t="n">
         <v>1</v>
@@ -10918,7 +10918,7 @@
         </is>
       </c>
       <c r="G168" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H168" t="n">
         <v>0</v>
@@ -11044,7 +11044,7 @@
         </is>
       </c>
       <c r="G170" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H170" t="n">
         <v>0</v>
@@ -11107,7 +11107,7 @@
         </is>
       </c>
       <c r="G171" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H171" t="n">
         <v>1</v>
@@ -11170,7 +11170,7 @@
         </is>
       </c>
       <c r="G172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H172" t="n">
         <v>2</v>
@@ -11179,13 +11179,13 @@
         <v>0</v>
       </c>
       <c r="J172" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L172" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M172" t="n">
         <v>0</v>
@@ -11231,7 +11231,7 @@
         </is>
       </c>
       <c r="G173" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H173" t="n">
         <v>3</v>
@@ -11240,13 +11240,13 @@
         <v>0</v>
       </c>
       <c r="J173" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L173" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M173" t="n">
         <v>0</v>
@@ -11292,25 +11292,25 @@
         </is>
       </c>
       <c r="G174" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H174" t="n">
         <v>1</v>
       </c>
       <c r="I174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J174" t="n">
         <v>0</v>
       </c>
       <c r="K174" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L174" t="n">
         <v>0</v>
       </c>
       <c r="M174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N174" t="n">
         <v>0</v>
@@ -11355,7 +11355,7 @@
         </is>
       </c>
       <c r="G175" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H175" t="n">
         <v>0</v>
@@ -11794,7 +11794,7 @@
         </is>
       </c>
       <c r="G182" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H182" t="n">
         <v>2</v>
@@ -11803,13 +11803,13 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K182" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M182" t="n">
         <v>0</v>
@@ -11857,7 +11857,7 @@
         </is>
       </c>
       <c r="G183" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H183" t="n">
         <v>4</v>
@@ -12353,7 +12353,7 @@
         </is>
       </c>
       <c r="G191" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H191" t="n">
         <v>4</v>
@@ -12542,7 +12542,7 @@
         </is>
       </c>
       <c r="G194" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H194" t="n">
         <v>3</v>
@@ -12668,7 +12668,7 @@
         </is>
       </c>
       <c r="G196" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H196" t="n">
         <v>0</v>
@@ -12857,25 +12857,25 @@
         </is>
       </c>
       <c r="G199" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H199" t="n">
         <v>1</v>
       </c>
       <c r="I199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J199" t="n">
         <v>0</v>
       </c>
       <c r="K199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L199" t="n">
         <v>0</v>
       </c>
       <c r="M199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N199" t="n">
         <v>0</v>
@@ -12920,7 +12920,7 @@
         </is>
       </c>
       <c r="G200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H200" t="n">
         <v>2</v>
@@ -12929,13 +12929,13 @@
         <v>0</v>
       </c>
       <c r="J200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M200" t="n">
         <v>0</v>
@@ -13235,7 +13235,7 @@
         </is>
       </c>
       <c r="G205" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H205" t="n">
         <v>0</v>
@@ -13298,25 +13298,25 @@
         </is>
       </c>
       <c r="G206" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H206" t="n">
         <v>1</v>
       </c>
       <c r="I206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J206" t="n">
         <v>0</v>
       </c>
       <c r="K206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L206" t="n">
         <v>0</v>
       </c>
       <c r="M206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N206" t="n">
         <v>0</v>
@@ -13359,7 +13359,7 @@
         </is>
       </c>
       <c r="G207" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H207" t="n">
         <v>0</v>
@@ -13733,7 +13733,7 @@
         </is>
       </c>
       <c r="G213" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H213" t="n">
         <v>2</v>
@@ -13742,13 +13742,13 @@
         <v>0</v>
       </c>
       <c r="J213" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K213" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L213" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M213" t="n">
         <v>0</v>
@@ -13859,7 +13859,7 @@
         </is>
       </c>
       <c r="G215" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H215" t="n">
         <v>0</v>
@@ -13985,7 +13985,7 @@
         </is>
       </c>
       <c r="G217" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H217" t="n">
         <v>0</v>
@@ -14172,7 +14172,7 @@
         </is>
       </c>
       <c r="G220" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H220" t="n">
         <v>1</v>
@@ -14235,25 +14235,25 @@
         </is>
       </c>
       <c r="G221" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H221" t="n">
         <v>3</v>
       </c>
       <c r="I221" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J221" t="n">
         <v>0</v>
       </c>
       <c r="K221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L221" t="n">
         <v>0</v>
       </c>
       <c r="M221" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N221" t="n">
         <v>-4</v>
@@ -14422,25 +14422,25 @@
         </is>
       </c>
       <c r="G224" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H224" t="n">
         <v>1</v>
       </c>
       <c r="I224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J224" t="n">
         <v>0</v>
       </c>
       <c r="K224" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L224" t="n">
         <v>0</v>
       </c>
       <c r="M224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N224" t="n">
         <v>0</v>
@@ -15298,25 +15298,25 @@
         </is>
       </c>
       <c r="G238" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H238" t="n">
         <v>1</v>
       </c>
       <c r="I238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J238" t="n">
         <v>0</v>
       </c>
       <c r="K238" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L238" t="n">
         <v>0</v>
       </c>
       <c r="M238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N238" t="n">
         <v>1</v>
@@ -15424,25 +15424,25 @@
         </is>
       </c>
       <c r="G240" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H240" t="n">
         <v>1</v>
       </c>
       <c r="I240" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J240" t="n">
         <v>0</v>
       </c>
       <c r="K240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L240" t="n">
         <v>0</v>
       </c>
       <c r="M240" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N240" t="n">
         <v>1</v>
@@ -15487,7 +15487,7 @@
         </is>
       </c>
       <c r="G241" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H241" t="n">
         <v>0</v>
@@ -15611,7 +15611,7 @@
         </is>
       </c>
       <c r="G243" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H243" t="n">
         <v>2</v>
@@ -15620,13 +15620,13 @@
         <v>0</v>
       </c>
       <c r="J243" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K243" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L243" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M243" t="n">
         <v>0</v>
@@ -15674,25 +15674,25 @@
         </is>
       </c>
       <c r="G244" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H244" t="n">
         <v>2</v>
       </c>
       <c r="I244" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J244" t="n">
         <v>0</v>
       </c>
       <c r="K244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L244" t="n">
         <v>0</v>
       </c>
       <c r="M244" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N244" t="n">
         <v>0</v>
@@ -15737,7 +15737,7 @@
         </is>
       </c>
       <c r="G245" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H245" t="n">
         <v>0</v>
@@ -15987,25 +15987,25 @@
         </is>
       </c>
       <c r="G249" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H249" t="n">
         <v>1</v>
       </c>
       <c r="I249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J249" t="n">
         <v>0</v>
       </c>
       <c r="K249" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L249" t="n">
         <v>0</v>
       </c>
       <c r="M249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N249" t="n">
         <v>-1</v>
@@ -16113,7 +16113,7 @@
         </is>
       </c>
       <c r="G251" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H251" t="n">
         <v>1</v>
@@ -16552,7 +16552,7 @@
         </is>
       </c>
       <c r="G258" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H258" t="n">
         <v>3</v>
@@ -16867,7 +16867,7 @@
         </is>
       </c>
       <c r="G263" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H263" t="n">
         <v>0</v>
@@ -16930,25 +16930,25 @@
         </is>
       </c>
       <c r="G264" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H264" t="n">
         <v>1</v>
       </c>
       <c r="I264" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J264" t="n">
         <v>0</v>
       </c>
       <c r="K264" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L264" t="n">
         <v>0</v>
       </c>
       <c r="M264" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N264" t="n">
         <v>2</v>
@@ -17430,25 +17430,25 @@
         </is>
       </c>
       <c r="G272" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H272" t="n">
         <v>1</v>
       </c>
       <c r="I272" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J272" t="n">
         <v>0</v>
       </c>
       <c r="K272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L272" t="n">
         <v>0</v>
       </c>
       <c r="M272" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N272" t="n">
         <v>2</v>
@@ -17556,7 +17556,7 @@
         </is>
       </c>
       <c r="G274" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H274" t="n">
         <v>2</v>
@@ -17743,25 +17743,25 @@
         </is>
       </c>
       <c r="G277" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H277" t="n">
         <v>2</v>
       </c>
       <c r="I277" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J277" t="n">
         <v>0</v>
       </c>
       <c r="K277" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L277" t="n">
         <v>0</v>
       </c>
       <c r="M277" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N277" t="n">
         <v>-1</v>
@@ -17867,7 +17867,7 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H279" t="n">
         <v>2</v>
@@ -17876,13 +17876,13 @@
         <v>0</v>
       </c>
       <c r="J279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K279" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M279" t="n">
         <v>0</v>
@@ -18054,7 +18054,7 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H282" t="n">
         <v>1</v>
@@ -18556,25 +18556,25 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H290" t="n">
         <v>1</v>
       </c>
       <c r="I290" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J290" t="n">
         <v>0</v>
       </c>
       <c r="K290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L290" t="n">
         <v>0</v>
       </c>
       <c r="M290" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N290" t="n">
         <v>1</v>
@@ -18743,25 +18743,25 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H293" t="n">
         <v>1</v>
       </c>
       <c r="I293" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J293" t="n">
         <v>0</v>
       </c>
       <c r="K293" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L293" t="n">
         <v>0</v>
       </c>
       <c r="M293" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N293" t="n">
         <v>0</v>
@@ -18930,7 +18930,7 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H296" t="n">
         <v>1</v>
@@ -19182,7 +19182,7 @@
         </is>
       </c>
       <c r="G300" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H300" t="n">
         <v>0</v>
@@ -19245,7 +19245,7 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H301" t="n">
         <v>2</v>
@@ -19747,7 +19747,7 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H309" t="n">
         <v>2</v>
@@ -19756,13 +19756,13 @@
         <v>0</v>
       </c>
       <c r="J309" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L309" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M309" t="n">
         <v>0</v>
@@ -20125,25 +20125,25 @@
         </is>
       </c>
       <c r="G315" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H315" t="n">
         <v>1</v>
       </c>
       <c r="I315" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J315" t="n">
         <v>0</v>
       </c>
       <c r="K315" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L315" t="n">
         <v>0</v>
       </c>
       <c r="M315" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N315" t="n">
         <v>1</v>
@@ -20188,7 +20188,7 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H316" t="n">
         <v>3</v>
@@ -20377,25 +20377,25 @@
         </is>
       </c>
       <c r="G319" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H319" t="n">
         <v>1</v>
       </c>
       <c r="I319" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J319" t="n">
         <v>0</v>
       </c>
       <c r="K319" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L319" t="n">
         <v>0</v>
       </c>
       <c r="M319" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N319" t="n">
         <v>-1</v>
@@ -20564,7 +20564,7 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H322" t="n">
         <v>2</v>
@@ -20573,13 +20573,13 @@
         <v>0</v>
       </c>
       <c r="J322" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K322" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L322" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M322" t="n">
         <v>0</v>
@@ -20690,7 +20690,7 @@
         </is>
       </c>
       <c r="G324" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H324" t="n">
         <v>3</v>
@@ -20753,25 +20753,25 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H325" t="n">
         <v>1</v>
       </c>
       <c r="I325" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J325" t="n">
         <v>0</v>
       </c>
       <c r="K325" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L325" t="n">
         <v>0</v>
       </c>
       <c r="M325" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N325" t="n">
         <v>0</v>
@@ -20816,25 +20816,25 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H326" t="n">
         <v>1</v>
       </c>
       <c r="I326" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J326" t="n">
         <v>0</v>
       </c>
       <c r="K326" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L326" t="n">
         <v>0</v>
       </c>
       <c r="M326" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N326" t="n">
         <v>6</v>
@@ -20940,25 +20940,25 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H328" t="n">
         <v>1</v>
       </c>
       <c r="I328" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J328" t="n">
         <v>0</v>
       </c>
       <c r="K328" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L328" t="n">
         <v>0</v>
       </c>
       <c r="M328" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N328" t="n">
         <v>2</v>
@@ -21001,7 +21001,7 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H329" t="n">
         <v>1</v>
@@ -21680,7 +21680,7 @@
         </is>
       </c>
       <c r="G340" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H340" t="n">
         <v>3</v>
@@ -21806,25 +21806,25 @@
         </is>
       </c>
       <c r="G342" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H342" t="n">
         <v>1</v>
       </c>
       <c r="I342" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J342" t="n">
         <v>0</v>
       </c>
       <c r="K342" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L342" t="n">
         <v>0</v>
       </c>
       <c r="M342" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N342" t="n">
         <v>-1</v>
@@ -21867,25 +21867,25 @@
         </is>
       </c>
       <c r="G343" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H343" t="n">
         <v>1</v>
       </c>
       <c r="I343" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J343" t="n">
         <v>0</v>
       </c>
       <c r="K343" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L343" t="n">
         <v>0</v>
       </c>
       <c r="M343" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N343" t="n">
         <v>-1</v>
@@ -22115,7 +22115,7 @@
         </is>
       </c>
       <c r="G347" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H347" t="n">
         <v>3</v>
@@ -22178,7 +22178,7 @@
         </is>
       </c>
       <c r="G348" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H348" t="n">
         <v>2</v>
@@ -22187,13 +22187,13 @@
         <v>0</v>
       </c>
       <c r="J348" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K348" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L348" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M348" t="n">
         <v>0</v>
@@ -22603,25 +22603,25 @@
         </is>
       </c>
       <c r="G355" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H355" t="n">
         <v>1</v>
       </c>
       <c r="I355" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J355" t="n">
         <v>0</v>
       </c>
       <c r="K355" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L355" t="n">
         <v>0</v>
       </c>
       <c r="M355" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N355" t="n">
         <v>-3</v>
@@ -22961,7 +22961,7 @@
         </is>
       </c>
       <c r="G361" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H361" t="n">
         <v>2</v>
@@ -22970,13 +22970,13 @@
         <v>0</v>
       </c>
       <c r="J361" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K361" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L361" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M361" t="n">
         <v>0</v>
@@ -23197,25 +23197,25 @@
         </is>
       </c>
       <c r="G365" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H365" t="n">
         <v>1</v>
       </c>
       <c r="I365" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J365" t="n">
         <v>0</v>
       </c>
       <c r="K365" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L365" t="n">
         <v>0</v>
       </c>
       <c r="M365" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N365" t="n">
         <v>-1</v>
@@ -23256,25 +23256,25 @@
         </is>
       </c>
       <c r="G366" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H366" t="n">
         <v>1</v>
       </c>
       <c r="I366" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J366" t="n">
         <v>0</v>
       </c>
       <c r="K366" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L366" t="n">
         <v>0</v>
       </c>
       <c r="M366" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N366" t="n">
         <v>1</v>
@@ -23317,7 +23317,7 @@
         </is>
       </c>
       <c r="G367" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H367" t="n">
         <v>2</v>
@@ -23326,13 +23326,13 @@
         <v>0</v>
       </c>
       <c r="J367" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K367" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L367" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M367" t="n">
         <v>0</v>
@@ -23553,7 +23553,7 @@
         </is>
       </c>
       <c r="G371" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H371" t="n">
         <v>3</v>
@@ -23612,25 +23612,25 @@
         </is>
       </c>
       <c r="G372" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H372" t="n">
         <v>1</v>
       </c>
       <c r="I372" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J372" t="n">
         <v>0</v>
       </c>
       <c r="K372" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L372" t="n">
         <v>0</v>
       </c>
       <c r="M372" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N372" t="n">
         <v>0</v>
@@ -23730,25 +23730,25 @@
         </is>
       </c>
       <c r="G374" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H374" t="n">
         <v>1</v>
       </c>
       <c r="I374" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J374" t="n">
         <v>0</v>
       </c>
       <c r="K374" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L374" t="n">
         <v>0</v>
       </c>
       <c r="M374" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N374" t="n">
         <v>1</v>
@@ -24027,25 +24027,25 @@
         </is>
       </c>
       <c r="G379" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H379" t="n">
         <v>1</v>
       </c>
       <c r="I379" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J379" t="n">
         <v>0</v>
       </c>
       <c r="K379" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L379" t="n">
         <v>0</v>
       </c>
       <c r="M379" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N379" t="n">
         <v>3</v>
@@ -24086,7 +24086,7 @@
         </is>
       </c>
       <c r="G380" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H380" t="n">
         <v>0</v>
@@ -24265,25 +24265,25 @@
         </is>
       </c>
       <c r="G383" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H383" t="n">
         <v>1</v>
       </c>
       <c r="I383" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J383" t="n">
         <v>0</v>
       </c>
       <c r="K383" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L383" t="n">
         <v>0</v>
       </c>
       <c r="M383" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N383" t="n">
         <v>1</v>
@@ -24324,7 +24324,7 @@
         </is>
       </c>
       <c r="G384" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H384" t="n">
         <v>3</v>
@@ -24442,7 +24442,7 @@
         </is>
       </c>
       <c r="G386" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H386" t="n">
         <v>2</v>
@@ -24451,13 +24451,13 @@
         <v>0</v>
       </c>
       <c r="J386" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K386" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L386" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M386" t="n">
         <v>0</v>
@@ -24560,7 +24560,7 @@
         </is>
       </c>
       <c r="G388" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H388" t="n">
         <v>2</v>
@@ -24569,13 +24569,13 @@
         <v>0</v>
       </c>
       <c r="J388" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K388" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L388" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M388" t="n">
         <v>0</v>
@@ -24975,7 +24975,7 @@
         </is>
       </c>
       <c r="G395" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H395" t="n">
         <v>2</v>
@@ -24984,13 +24984,13 @@
         <v>0</v>
       </c>
       <c r="J395" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K395" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L395" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M395" t="n">
         <v>0</v>
@@ -25152,25 +25152,25 @@
         </is>
       </c>
       <c r="G398" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H398" t="n">
         <v>1</v>
       </c>
       <c r="I398" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J398" t="n">
         <v>0</v>
       </c>
       <c r="K398" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L398" t="n">
         <v>0</v>
       </c>
       <c r="M398" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N398" t="n">
         <v>0</v>
@@ -25506,7 +25506,7 @@
         </is>
       </c>
       <c r="G404" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H404" t="n">
         <v>0</v>
@@ -26393,7 +26393,7 @@
         </is>
       </c>
       <c r="G419" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H419" t="n">
         <v>1</v>
@@ -26452,7 +26452,7 @@
         </is>
       </c>
       <c r="G420" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H420" t="n">
         <v>1</v>
@@ -26511,25 +26511,25 @@
         </is>
       </c>
       <c r="G421" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H421" t="n">
         <v>2</v>
       </c>
       <c r="I421" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J421" t="n">
         <v>0</v>
       </c>
       <c r="K421" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L421" t="n">
         <v>0</v>
       </c>
       <c r="M421" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N421" t="n">
         <v>4</v>
@@ -26629,25 +26629,25 @@
         </is>
       </c>
       <c r="G423" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H423" t="n">
         <v>3</v>
       </c>
       <c r="I423" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J423" t="n">
         <v>0</v>
       </c>
       <c r="K423" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L423" t="n">
         <v>0</v>
       </c>
       <c r="M423" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N423" t="n">
         <v>-4</v>
@@ -26688,25 +26688,25 @@
         </is>
       </c>
       <c r="G424" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H424" t="n">
         <v>1</v>
       </c>
       <c r="I424" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J424" t="n">
         <v>0</v>
       </c>
       <c r="K424" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L424" t="n">
         <v>0</v>
       </c>
       <c r="M424" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N424" t="n">
         <v>0</v>
@@ -26806,7 +26806,7 @@
         </is>
       </c>
       <c r="G426" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H426" t="n">
         <v>1</v>
@@ -26865,7 +26865,7 @@
         </is>
       </c>
       <c r="G427" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H427" t="n">
         <v>2</v>
@@ -27514,25 +27514,25 @@
         </is>
       </c>
       <c r="G438" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H438" t="n">
         <v>1</v>
       </c>
       <c r="I438" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J438" t="n">
         <v>0</v>
       </c>
       <c r="K438" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L438" t="n">
         <v>0</v>
       </c>
       <c r="M438" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N438" t="n">
         <v>3</v>
@@ -27691,7 +27691,7 @@
         </is>
       </c>
       <c r="G441" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H441" t="n">
         <v>2</v>
@@ -27700,13 +27700,13 @@
         <v>0</v>
       </c>
       <c r="J441" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K441" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L441" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M441" t="n">
         <v>0</v>
@@ -27868,7 +27868,7 @@
         </is>
       </c>
       <c r="G444" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H444" t="n">
         <v>0</v>
@@ -27927,7 +27927,7 @@
         </is>
       </c>
       <c r="G445" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H445" t="n">
         <v>2</v>
@@ -27936,13 +27936,13 @@
         <v>0</v>
       </c>
       <c r="J445" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K445" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L445" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M445" t="n">
         <v>0</v>
@@ -27986,7 +27986,7 @@
         </is>
       </c>
       <c r="G446" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H446" t="n">
         <v>0</v>
@@ -28163,25 +28163,25 @@
         </is>
       </c>
       <c r="G449" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H449" t="n">
         <v>1</v>
       </c>
       <c r="I449" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J449" t="n">
         <v>0</v>
       </c>
       <c r="K449" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L449" t="n">
         <v>0</v>
       </c>
       <c r="M449" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N449" t="n">
         <v>2</v>
@@ -28222,7 +28222,7 @@
         </is>
       </c>
       <c r="G450" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H450" t="n">
         <v>2</v>
@@ -28231,13 +28231,13 @@
         <v>0</v>
       </c>
       <c r="J450" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K450" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L450" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M450" t="n">
         <v>0</v>
@@ -28340,7 +28340,7 @@
         </is>
       </c>
       <c r="G452" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H452" t="n">
         <v>2</v>
@@ -28349,13 +28349,13 @@
         <v>0</v>
       </c>
       <c r="J452" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K452" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L452" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M452" t="n">
         <v>0</v>
@@ -28517,25 +28517,25 @@
         </is>
       </c>
       <c r="G455" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H455" t="n">
         <v>1</v>
       </c>
       <c r="I455" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J455" t="n">
         <v>0</v>
       </c>
       <c r="K455" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L455" t="n">
         <v>0</v>
       </c>
       <c r="M455" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N455" t="n">
         <v>0</v>
@@ -28576,25 +28576,25 @@
         </is>
       </c>
       <c r="G456" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H456" t="n">
         <v>1</v>
       </c>
       <c r="I456" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J456" t="n">
         <v>0</v>
       </c>
       <c r="K456" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L456" t="n">
         <v>0</v>
       </c>
       <c r="M456" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N456" t="n">
         <v>2</v>
@@ -28694,7 +28694,7 @@
         </is>
       </c>
       <c r="G458" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H458" t="n">
         <v>2</v>
@@ -28703,13 +28703,13 @@
         <v>0</v>
       </c>
       <c r="J458" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K458" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L458" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M458" t="n">
         <v>0</v>
@@ -28812,25 +28812,25 @@
         </is>
       </c>
       <c r="G460" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H460" t="n">
         <v>1</v>
       </c>
       <c r="I460" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J460" t="n">
         <v>0</v>
       </c>
       <c r="K460" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L460" t="n">
         <v>0</v>
       </c>
       <c r="M460" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N460" t="n">
         <v>2</v>
@@ -29048,25 +29048,25 @@
         </is>
       </c>
       <c r="G464" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H464" t="n">
         <v>1</v>
       </c>
       <c r="I464" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J464" t="n">
         <v>0</v>
       </c>
       <c r="K464" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L464" t="n">
         <v>0</v>
       </c>
       <c r="M464" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N464" t="n">
         <v>0</v>
@@ -29166,7 +29166,7 @@
         </is>
       </c>
       <c r="G466" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H466" t="n">
         <v>2</v>
@@ -29175,13 +29175,13 @@
         <v>0</v>
       </c>
       <c r="J466" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K466" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L466" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M466" t="n">
         <v>0</v>
@@ -29225,7 +29225,7 @@
         </is>
       </c>
       <c r="G467" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H467" t="n">
         <v>2</v>
@@ -29234,13 +29234,13 @@
         <v>0</v>
       </c>
       <c r="J467" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K467" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L467" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M467" t="n">
         <v>0</v>
@@ -29284,7 +29284,7 @@
         </is>
       </c>
       <c r="G468" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H468" t="n">
         <v>2</v>
@@ -29293,13 +29293,13 @@
         <v>0</v>
       </c>
       <c r="J468" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K468" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L468" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M468" t="n">
         <v>0</v>
@@ -29520,7 +29520,7 @@
         </is>
       </c>
       <c r="G472" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H472" t="n">
         <v>1</v>
@@ -29529,13 +29529,13 @@
         <v>0</v>
       </c>
       <c r="J472" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K472" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L472" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M472" t="n">
         <v>0</v>
@@ -29579,7 +29579,7 @@
         </is>
       </c>
       <c r="G473" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H473" t="n">
         <v>4</v>
@@ -30346,25 +30346,25 @@
         </is>
       </c>
       <c r="G486" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H486" t="n">
         <v>1</v>
       </c>
       <c r="I486" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J486" t="n">
         <v>0</v>
       </c>
       <c r="K486" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L486" t="n">
         <v>0</v>
       </c>
       <c r="M486" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N486" t="n">
         <v>3</v>
@@ -30818,7 +30818,7 @@
         </is>
       </c>
       <c r="G494" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H494" t="n">
         <v>2</v>
@@ -30827,13 +30827,13 @@
         <v>0</v>
       </c>
       <c r="J494" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K494" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L494" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M494" t="n">
         <v>0</v>
@@ -30995,25 +30995,25 @@
         </is>
       </c>
       <c r="G497" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H497" t="n">
         <v>1</v>
       </c>
       <c r="I497" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J497" t="n">
         <v>0</v>
       </c>
       <c r="K497" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L497" t="n">
         <v>0</v>
       </c>
       <c r="M497" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N497" t="n">
         <v>2</v>
@@ -31172,25 +31172,25 @@
         </is>
       </c>
       <c r="G500" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H500" t="n">
         <v>1</v>
       </c>
       <c r="I500" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J500" t="n">
         <v>0</v>
       </c>
       <c r="K500" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L500" t="n">
         <v>0</v>
       </c>
       <c r="M500" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N500" t="n">
         <v>1</v>
@@ -31526,7 +31526,7 @@
         </is>
       </c>
       <c r="G506" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H506" t="n">
         <v>0</v>
@@ -31762,7 +31762,7 @@
         </is>
       </c>
       <c r="G510" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H510" t="n">
         <v>2</v>
@@ -31771,13 +31771,13 @@
         <v>0</v>
       </c>
       <c r="J510" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K510" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L510" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M510" t="n">
         <v>0</v>
@@ -31880,7 +31880,7 @@
         </is>
       </c>
       <c r="G512" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H512" t="n">
         <v>2</v>
@@ -31889,13 +31889,13 @@
         <v>0</v>
       </c>
       <c r="J512" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K512" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L512" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M512" t="n">
         <v>0</v>
@@ -32470,7 +32470,7 @@
         </is>
       </c>
       <c r="G522" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H522" t="n">
         <v>2</v>
@@ -32479,13 +32479,13 @@
         <v>0</v>
       </c>
       <c r="J522" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K522" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L522" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M522" t="n">
         <v>0</v>
@@ -32765,7 +32765,7 @@
         </is>
       </c>
       <c r="G527" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H527" t="n">
         <v>0</v>
@@ -33001,25 +33001,25 @@
         </is>
       </c>
       <c r="G531" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H531" t="n">
         <v>1</v>
       </c>
       <c r="I531" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J531" t="n">
         <v>0</v>
       </c>
       <c r="K531" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L531" t="n">
         <v>0</v>
       </c>
       <c r="M531" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N531" t="n">
         <v>1</v>
@@ -33178,7 +33178,7 @@
         </is>
       </c>
       <c r="G534" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H534" t="n">
         <v>2</v>
@@ -33187,13 +33187,13 @@
         <v>0</v>
       </c>
       <c r="J534" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K534" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L534" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M534" t="n">
         <v>0</v>
@@ -34771,25 +34771,25 @@
         </is>
       </c>
       <c r="G561" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H561" t="n">
         <v>1</v>
       </c>
       <c r="I561" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J561" t="n">
         <v>0</v>
       </c>
       <c r="K561" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L561" t="n">
         <v>0</v>
       </c>
       <c r="M561" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N561" t="n">
         <v>-3</v>

</xml_diff>